<commit_message>
Added new viruses from fish, and Mengla virus
</commit_message>
<xml_diff>
--- a/tabular/ebola-ncbi-refseqs-side-data.xlsx
+++ b/tabular/ebola-ncbi-refseqs-side-data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
   <si>
     <t xml:space="preserve">NC_001608 </t>
   </si>
@@ -134,13 +134,58 @@
   </si>
   <si>
     <t>NC_001608</t>
+  </si>
+  <si>
+    <t>KX371887</t>
+  </si>
+  <si>
+    <t>MG599980</t>
+  </si>
+  <si>
+    <t>MG599981</t>
+  </si>
+  <si>
+    <t>Mengla</t>
+  </si>
+  <si>
+    <t>Xilang</t>
+  </si>
+  <si>
+    <t>Huangjiao</t>
+  </si>
+  <si>
+    <t>MLAV</t>
+  </si>
+  <si>
+    <t>XILV</t>
+  </si>
+  <si>
+    <t>HUJV</t>
+  </si>
+  <si>
+    <t>Dianlovirus</t>
+  </si>
+  <si>
+    <t>Striavirus</t>
+  </si>
+  <si>
+    <t>Thamnovirus</t>
+  </si>
+  <si>
+    <t>RAVV</t>
+  </si>
+  <si>
+    <t>DQ447649</t>
+  </si>
+  <si>
+    <t>Lake Victoria marburgvirus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -191,8 +236,14 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -244,6 +295,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF20FFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0F80FF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000080"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -257,7 +326,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="63">
+  <cellStyleXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -321,8 +390,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -333,8 +408,11 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="63">
+  <cellStyles count="69">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -366,6 +444,9 @@
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -397,6 +478,9 @@
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -726,17 +810,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="A2:D9"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.83203125" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27.5" customWidth="1"/>
     <col min="4" max="4" width="47.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -864,6 +948,62 @@
       </c>
       <c r="D9" s="7" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18">
+      <c r="A10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="18">
+      <c r="A11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="18">
+      <c r="A12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="18">
+      <c r="A13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>